<commit_message>
Login Funcional, Listado de productos version basica
</commit_message>
<xml_diff>
--- a/ProyectoSemestreWeb/Requerimientos Proyecto.xlsx
+++ b/ProyectoSemestreWeb/Requerimientos Proyecto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://profesoresuniajcedu-my.sharepoint.com/personal/cristiandlopez_estudiante_uniajc_edu_co/Documents/Universidad/Fundamentos Web/ProyectoSemestreWeb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="50" documentId="8_{734A9C99-6CDA-4D18-BD0F-D8684CA19849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F61EA510-30DF-4F58-88AC-A815033B75C9}"/>
+  <xr:revisionPtr revIDLastSave="53" documentId="8_{734A9C99-6CDA-4D18-BD0F-D8684CA19849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72FCC5F3-F9F9-4051-B9E1-E9D007D02F6C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8DAC96EC-DC58-4460-A069-A9D1CE29242F}"/>
   </bookViews>
@@ -566,7 +566,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2D9E3A6-8223-49F2-BA59-B1B449ADF441}">
   <dimension ref="A3:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -745,7 +745,7 @@
       </c>
     </row>
     <row r="21" spans="2:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="4" t="s">
         <v>37</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -753,7 +753,7 @@
       </c>
     </row>
     <row r="22" spans="2:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="4" t="s">
         <v>38</v>
       </c>
       <c r="C22" s="3" t="s">
@@ -761,7 +761,7 @@
       </c>
     </row>
     <row r="23" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="4" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>